<commit_message>
Increase MCGLT to hit 1.5 target
</commit_message>
<xml_diff>
--- a/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
+++ b/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
@@ -416,7 +416,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -520,7 +520,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1557,7 +1557,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1592,11 +1592,11 @@
         <v>118</v>
       </c>
       <c r="C2" s="13">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D2" s="13">
         <f>C2</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.45">
@@ -1619,11 +1619,11 @@
         <v>118</v>
       </c>
       <c r="C4" s="13">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D4" s="13">
         <f>C4</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.45">
@@ -1646,11 +1646,11 @@
         <v>118</v>
       </c>
       <c r="C6" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D6" s="11">
         <f>C6</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.45">
@@ -1673,11 +1673,11 @@
         <v>118</v>
       </c>
       <c r="C8" s="13">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D8" s="11">
         <f>C8</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1715,11 +1715,11 @@
         <v>118</v>
       </c>
       <c r="C10" s="5">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D10" s="13">
         <f>C10</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1782,11 +1782,11 @@
         <v>118</v>
       </c>
       <c r="C12" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D12" s="13">
         <f>C12</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
@@ -1876,11 +1876,11 @@
         <v>118</v>
       </c>
       <c r="C14" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D14" s="11">
         <f>C14</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.45">
@@ -1903,11 +1903,11 @@
         <v>118</v>
       </c>
       <c r="C16" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D16" s="11">
         <f>C16</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -1930,11 +1930,11 @@
         <v>118</v>
       </c>
       <c r="C18" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D18" s="11">
         <f>C18</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
@@ -1957,11 +1957,11 @@
         <v>118</v>
       </c>
       <c r="C20" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D20" s="11">
         <f>C20</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -1984,11 +1984,11 @@
         <v>118</v>
       </c>
       <c r="C22" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D22" s="11">
         <f>C22</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -2011,11 +2011,11 @@
         <v>118</v>
       </c>
       <c r="C24" s="13">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D24" s="5">
         <f>C24</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -2039,12 +2039,12 @@
         <v>118</v>
       </c>
       <c r="C26" s="13">
-        <f>IF(About!C2=1,500,0)</f>
-        <v>500</v>
+        <f>IF(About!C2=1,700,0)</f>
+        <v>700</v>
       </c>
       <c r="D26" s="13">
         <f>C26</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E26" s="8"/>
     </row>
@@ -2069,7 +2069,7 @@
         <v>118</v>
       </c>
       <c r="C28" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D28" s="11">
         <v>0</v>
@@ -2095,7 +2095,7 @@
         <v>118</v>
       </c>
       <c r="C30" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D30" s="11">
         <v>0</v>
@@ -2121,11 +2121,11 @@
         <v>118</v>
       </c>
       <c r="C32" s="11">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D32" s="11">
         <f>C32</f>
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>